<commit_message>
Push And Commit as on 04-May-2019.
</commit_message>
<xml_diff>
--- a/NwntTest/src/main/java/com/nwnt/qa/testdata/AssignAppointment.xlsx
+++ b/NwntTest/src/main/java/com/nwnt/qa/testdata/AssignAppointment.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15495" windowHeight="3225" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DoctorApp" sheetId="1" r:id="rId1"/>
     <sheet name="PanelApp" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>AppWith</t>
   </si>
@@ -416,7 +416,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,10 +505,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,11 +518,10 @@
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,13 +538,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -562,13 +558,22 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>